<commit_message>
Homepage: students in group can no longer see the "applied" tab
</commit_message>
<xml_diff>
--- a/docs/Permissions-1.2.xlsx
+++ b/docs/Permissions-1.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentxjtlueducn-my.sharepoint.com/personal/xian_he18_student_xjtlu_edu_cn/Documents/Year 3 Semester 2/CPT202 Software Engineering Group Project/docs/UI + Logic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lenovo\Documents\GitHub\CPT202_GMS\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{71DB2417-C7F0-4ADE-B845-70B27C16B126}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{97703BE2-1C6A-4509-A56C-F10EC3D48300}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB594E6-F95F-4A1A-BD05-6B8E8D082F63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5925" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{F51D6D4E-2AA4-483B-A341-8096C24954B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F51D6D4E-2AA4-483B-A341-8096C24954B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Homepage" sheetId="10" r:id="rId1"/>
@@ -1052,27 +1052,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2587C1B7-B1EA-4CC1-A87A-DEA2A57501D7}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.41015625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.76171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.29296875" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.234375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.52734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.76171875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.29296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.8203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.41015625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.52734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.234375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>73</v>
       </c>
@@ -1088,7 +1088,7 @@
       <c r="K1" s="13"/>
       <c r="L1" s="13"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
       <c r="B2" s="15"/>
       <c r="C2" s="12" t="s">
@@ -1110,7 +1110,7 @@
       </c>
       <c r="L2" s="18"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="16"/>
       <c r="B3" s="17"/>
       <c r="C3" s="3" t="s">
@@ -1144,7 +1144,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>59</v>
       </c>
@@ -1162,13 +1162,13 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="20"/>
       <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1178,13 +1178,13 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="20"/>
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -1194,7 +1194,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="21"/>
       <c r="B7" s="4" t="s">
         <v>17</v>
@@ -1231,22 +1231,22 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.76171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.41015625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.52734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.29296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5859375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.29296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.41015625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.9375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.9375" customWidth="1"/>
-    <col min="11" max="11" width="16.234375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="16.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1261,7 +1261,7 @@
       <c r="J1" s="13"/>
       <c r="K1" s="18"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23" t="s">
@@ -1284,7 +1284,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="3" t="s">
@@ -1315,7 +1315,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
         <v>15</v>
       </c>
@@ -1332,7 +1332,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="24"/>
       <c r="B5" s="4" t="s">
         <v>12</v>
@@ -1347,7 +1347,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="24"/>
       <c r="B6" s="4" t="s">
         <v>13</v>
@@ -1362,7 +1362,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="24"/>
       <c r="B7" s="4" t="s">
         <v>34</v>
@@ -1377,7 +1377,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
       <c r="B8" s="4" t="s">
         <v>17</v>
@@ -1392,7 +1392,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
         <v>14</v>
       </c>
@@ -1409,7 +1409,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="23"/>
       <c r="B10" s="4" t="s">
         <v>12</v>
@@ -1424,7 +1424,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="23"/>
       <c r="B11" s="4" t="s">
         <v>13</v>
@@ -1439,7 +1439,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="23"/>
       <c r="B12" s="4" t="s">
         <v>34</v>
@@ -1454,7 +1454,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="23"/>
       <c r="B13" s="4" t="s">
         <v>17</v>
@@ -1469,7 +1469,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
         <v>18</v>
       </c>
@@ -1486,7 +1486,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="23"/>
       <c r="B15" s="4" t="s">
         <v>13</v>
@@ -1501,7 +1501,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="23"/>
       <c r="B16" s="4" t="s">
         <v>34</v>
@@ -1516,7 +1516,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="23"/>
       <c r="B17" s="4" t="s">
         <v>17</v>
@@ -1531,7 +1531,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
         <v>84</v>
       </c>
@@ -1571,25 +1571,25 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.76171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.41015625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.29296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.8203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.05859375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5859375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.3515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.05859375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.05859375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.64453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.1171875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.76171875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.1171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>19</v>
       </c>
@@ -1607,7 +1607,7 @@
       <c r="M1" s="13"/>
       <c r="N1" s="18"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="6" t="s">
@@ -1631,7 +1631,7 @@
       <c r="M2" s="13"/>
       <c r="N2" s="18"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="3" t="s">
@@ -1671,7 +1671,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>15</v>
       </c>
@@ -1693,7 +1693,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="23"/>
       <c r="B5" s="3" t="s">
         <v>13</v>
@@ -1711,7 +1711,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="2"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="23"/>
       <c r="B6" s="3" t="s">
         <v>17</v>
@@ -1729,7 +1729,7 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>14</v>
       </c>
@@ -1755,7 +1755,7 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="23"/>
       <c r="B8" s="3" t="s">
         <v>13</v>
@@ -1773,7 +1773,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="3" t="s">
         <v>17</v>
@@ -1793,7 +1793,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
         <v>18</v>
       </c>
@@ -1819,7 +1819,7 @@
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="23"/>
       <c r="B11" s="3" t="s">
         <v>13</v>
@@ -1837,7 +1837,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="23"/>
       <c r="B12" s="3" t="s">
         <v>17</v>
@@ -1857,7 +1857,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
         <v>85</v>
       </c>
@@ -1899,16 +1899,16 @@
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.76171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.41015625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.05859375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.05859375" customWidth="1"/>
-    <col min="6" max="6" width="17.29296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13" customWidth="1"/>
+    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>23</v>
       </c>
@@ -1918,7 +1918,7 @@
       <c r="E1" s="26"/>
       <c r="F1" s="26"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="12" t="s">
@@ -1928,7 +1928,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="9" t="s">
@@ -1944,7 +1944,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>15</v>
       </c>
@@ -1956,7 +1956,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="23"/>
       <c r="B5" s="3" t="s">
         <v>17</v>
@@ -1966,7 +1966,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>14</v>
       </c>
@@ -1978,7 +1978,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="23"/>
       <c r="B7" s="3" t="s">
         <v>17</v>
@@ -1988,7 +1988,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>18</v>
       </c>
@@ -2000,7 +2000,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="3" t="s">
         <v>17</v>
@@ -2032,19 +2032,19 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.8203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.41015625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.64453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.52734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.41015625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.17578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.29296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.64453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>58</v>
       </c>
@@ -2056,7 +2056,7 @@
       <c r="G1" s="23"/>
       <c r="H1" s="23"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23" t="s">
@@ -2076,7 +2076,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="3" t="s">
@@ -2098,7 +2098,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>55</v>
       </c>
@@ -2112,7 +2112,7 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="23"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -2124,7 +2124,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="23"/>
       <c r="B6" s="3" t="s">
         <v>13</v>
@@ -2136,7 +2136,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="23"/>
       <c r="B7" s="3" t="s">
         <v>17</v>
@@ -2148,7 +2148,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>56</v>
       </c>
@@ -2162,7 +2162,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23"/>
       <c r="B9" s="3" t="s">
         <v>12</v>
@@ -2174,7 +2174,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="23"/>
       <c r="B10" s="3" t="s">
         <v>13</v>
@@ -2186,7 +2186,7 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="23"/>
       <c r="B11" s="3" t="s">
         <v>17</v>
@@ -2198,7 +2198,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
         <v>57</v>
       </c>
@@ -2212,7 +2212,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="23"/>
       <c r="B13" s="3" t="s">
         <v>13</v>
@@ -2224,7 +2224,7 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="23"/>
       <c r="B14" s="3" t="s">
         <v>17</v>
@@ -2258,17 +2258,17 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.41015625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.52734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.64453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>46</v>
       </c>
@@ -2278,7 +2278,7 @@
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="12" t="s">
@@ -2288,7 +2288,7 @@
       <c r="E2" s="13"/>
       <c r="F2" s="18"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="3" t="s">
@@ -2304,7 +2304,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>59</v>
       </c>
@@ -2316,7 +2316,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="23"/>
       <c r="B5" s="3" t="s">
         <v>12</v>
@@ -2326,7 +2326,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="23"/>
       <c r="B6" s="3" t="s">
         <v>13</v>
@@ -2336,7 +2336,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="23"/>
       <c r="B7" s="3" t="s">
         <v>17</v>
@@ -2362,24 +2362,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35BB35A3-CEA8-4DCA-B249-305B496325E5}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.8203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.05859375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.3515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.87890625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.64453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.9375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.76171875" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.1171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>52</v>
       </c>
@@ -2392,7 +2392,7 @@
       <c r="H1" s="23"/>
       <c r="I1" s="23"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="12" t="s">
@@ -2405,7 +2405,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="18"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="3" t="s">
@@ -2430,7 +2430,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>55</v>
       </c>
@@ -2453,7 +2453,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>56</v>
       </c>
@@ -2468,7 +2468,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>57</v>
       </c>
@@ -2502,15 +2502,15 @@
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5859375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.17578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>53</v>
       </c>
@@ -2518,7 +2518,7 @@
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="12" t="s">
@@ -2526,7 +2526,7 @@
       </c>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="3" t="s">
@@ -2536,7 +2536,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>59</v>
       </c>
@@ -2565,16 +2565,16 @@
       <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.64453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.05859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="s">
         <v>54</v>
       </c>
@@ -2583,7 +2583,7 @@
       <c r="D1" s="23"/>
       <c r="E1" s="23"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="12" t="s">
@@ -2592,7 +2592,7 @@
       <c r="D2" s="13"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="3" t="s">
@@ -2605,7 +2605,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>59</v>
       </c>

</xml_diff>